<commit_message>
Add 'last_updated' field to the Course model & make migrations
</commit_message>
<xml_diff>
--- a/data_sample.xlsx
+++ b/data_sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stanislavmayatsky/python/Skypro/module8/homework-33/school/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C55D2CF-C7AA-D540-AE84-E87241EF57E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA00B075-7FF9-684D-B3CD-A94B83BCEBBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="280" yWindow="500" windowWidth="28240" windowHeight="16340" xr2:uid="{2B6990DE-B248-9E4B-9354-089A929C6AC1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t>Course</t>
   </si>
@@ -83,15 +83,6 @@
     <t>Алгоритмы сортировки</t>
   </si>
   <si>
-    <t>2 lessons</t>
-  </si>
-  <si>
-    <t>1 lesson</t>
-  </si>
-  <si>
-    <t>0 lessons</t>
-  </si>
-  <si>
     <t>Payment</t>
   </si>
   <si>
@@ -146,17 +137,17 @@
     <t>null</t>
   </si>
   <si>
-    <t>Столбец1</t>
-  </si>
-  <si>
-    <t>Столбец2</t>
+    <t>owner_id</t>
+  </si>
+  <si>
+    <t>lessons_count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +175,14 @@
       <name val="SF Mono"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -205,16 +204,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -285,26 +300,6 @@
     </dxf>
     <dxf>
       <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color auto="1"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -319,6 +314,16 @@
         <name val="SF Mono"/>
         <family val="3"/>
         <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
       </font>
     </dxf>
     <dxf>
@@ -406,25 +411,25 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9AE70BDE-C6C6-2E46-BAFA-A21A5EB84DEA}" name="Таблица4" displayName="Таблица4" ref="B13:D18" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9AE70BDE-C6C6-2E46-BAFA-A21A5EB84DEA}" name="Таблица4" displayName="Таблица4" ref="B13:D18" totalsRowShown="0" dataDxfId="9">
   <autoFilter ref="B13:D18" xr:uid="{9AE70BDE-C6C6-2E46-BAFA-A21A5EB84DEA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{D06D8A6D-17DC-A54F-B231-097AC77F9C78}" name="id" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{B659CA8F-6010-904B-970C-E1EF94C81C64}" name="name" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{2D088223-F1F4-F04E-BC5A-7F4F1FCF4BC6}" name="course" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{D06D8A6D-17DC-A54F-B231-097AC77F9C78}" name="id" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{B659CA8F-6010-904B-970C-E1EF94C81C64}" name="name" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{2D088223-F1F4-F04E-BC5A-7F4F1FCF4BC6}" name="course" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium10" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C9768D5-BE55-5240-A972-BDD3DEE47730}" name="Таблица6" displayName="Таблица6" ref="B4:E9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{8C9768D5-BE55-5240-A972-BDD3DEE47730}" name="Таблица6" displayName="Таблица6" ref="B4:E9" totalsRowShown="0" headerRowDxfId="0" dataDxfId="5">
   <autoFilter ref="B4:E9" xr:uid="{8C9768D5-BE55-5240-A972-BDD3DEE47730}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{20720694-3A97-394B-8704-60B2248087B4}" name="id" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{3F43D6AF-AE69-804C-A9A6-0795AC1F0112}" name="name" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{FFE58E7C-3826-B642-BD54-C5928C48D5B9}" name="Столбец1" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{136ABB5B-D0A0-2E45-B7D0-303A2E9B007C}" name="Столбец2" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{20720694-3A97-394B-8704-60B2248087B4}" name="id" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{3F43D6AF-AE69-804C-A9A6-0795AC1F0112}" name="name" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{FFE58E7C-3826-B642-BD54-C5928C48D5B9}" name="owner_id" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{136ABB5B-D0A0-2E45-B7D0-303A2E9B007C}" name="lessons_count" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -750,7 +755,7 @@
   <dimension ref="B3:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -758,7 +763,7 @@
     <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="30.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.83203125" customWidth="1"/>
-    <col min="5" max="5" width="11.5" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:5">
@@ -767,17 +772,17 @@
       </c>
     </row>
     <row r="4" spans="2:5">
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>37</v>
+      <c r="B4" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -787,8 +792,12 @@
       <c r="C5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="D5" s="2">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="2:5">
       <c r="B6" s="2">
@@ -797,9 +806,11 @@
       <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>15</v>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -809,9 +820,11 @@
       <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2" t="s">
-        <v>16</v>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -821,9 +834,11 @@
       <c r="C8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2" t="s">
-        <v>16</v>
+      <c r="D8" s="2">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -833,9 +848,11 @@
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="2">
+        <v>4</v>
+      </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="2:5">
@@ -911,7 +928,7 @@
     </row>
     <row r="21" spans="2:5">
       <c r="B21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -919,10 +936,10 @@
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -930,10 +947,10 @@
         <v>1</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -941,10 +958,10 @@
         <v>2</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -952,10 +969,10 @@
         <v>3</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="2:5">
@@ -963,10 +980,10 @@
         <v>4</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="2:5">
@@ -974,15 +991,15 @@
         <v>5</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="2:5">
       <c r="B30" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="2:5">
@@ -990,13 +1007,13 @@
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="2:5">
@@ -1010,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="2:5">
@@ -1021,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E33">
         <v>3</v>
@@ -1038,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="E34" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="35" spans="2:5">
@@ -1049,7 +1066,7 @@
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1066,7 +1083,7 @@
         <v>3</v>
       </c>
       <c r="E36" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="2:5">
@@ -1080,7 +1097,7 @@
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="2:5">
@@ -1091,7 +1108,7 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E38">
         <v>2</v>
@@ -1105,7 +1122,7 @@
         <v>4</v>
       </c>
       <c r="D39" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E39">
         <v>5</v>
@@ -1119,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="D40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E40">
         <v>5</v>
@@ -1136,7 +1153,7 @@
         <v>2</v>
       </c>
       <c r="E41" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>